<commit_message>
local commit from mac
</commit_message>
<xml_diff>
--- a/results/xls/local-payload-no.xlsx
+++ b/results/xls/local-payload-no.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agabaisaac/iot/mist-framework/results/csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agabaisaac/iot/mist-framework/results/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="1980" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="local-payload-no.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -41,9 +41,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>Results</t>
-  </si>
-  <si>
     <t>8rfjc</t>
   </si>
   <si>
@@ -108,13 +105,22 @@
   </si>
   <si>
     <t>pqM2l</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 2 Results </t>
+  </si>
+  <si>
+    <t>Test 1 Results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,13 +128,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,8 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,15 +456,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:T124"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113:XFD113"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="3.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,1550 +482,2046 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>1490726265360</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>1490726265574</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <f>(D3-D2)/1000</f>
+        <v>0.214</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>0.214</v>
+      </c>
+      <c r="J3">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="K3">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="L3">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="M3">
+        <v>0.222</v>
+      </c>
+      <c r="N3" s="4">
+        <f>AVERAGE(I3:M3)</f>
+        <v>0.20800000000000002</v>
+      </c>
+      <c r="O3">
+        <v>2.117</v>
+      </c>
+      <c r="P3">
+        <v>0.217</v>
+      </c>
+      <c r="Q3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R3">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="S3">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="T3" s="1">
+        <f>AVERAGE(O3:S3)</f>
+        <v>0.59079999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1490726265927</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>1490726343864</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f>(D5-D4)/1000</f>
+        <v>77.936999999999998</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>77.936999999999998</v>
+      </c>
+      <c r="J5">
+        <v>6.0570000000000004</v>
+      </c>
+      <c r="K5">
+        <v>6.0640000000000001</v>
+      </c>
+      <c r="L5">
+        <v>6.5350000000000001</v>
+      </c>
+      <c r="M5">
+        <v>6.3109999999999999</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" ref="N5:N11" si="0">AVERAGE(I5:M5)</f>
+        <v>20.5808</v>
+      </c>
+      <c r="O5">
+        <v>42.241999999999997</v>
+      </c>
+      <c r="P5">
+        <v>6.0090000000000003</v>
+      </c>
+      <c r="Q5">
+        <v>6.3150000000000004</v>
+      </c>
+      <c r="R5">
+        <v>5.444</v>
+      </c>
+      <c r="S5">
+        <v>7.57</v>
+      </c>
+      <c r="T5" s="1">
+        <f t="shared" ref="T5:T11" si="1">AVERAGE(O5:S5)</f>
+        <v>13.516</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>1490726345417</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>1490726357660</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f>(D7-D6)/1000</f>
+        <v>12.243</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>12.243</v>
+      </c>
+      <c r="J7">
+        <v>17.922999999999998</v>
+      </c>
+      <c r="K7">
+        <v>18.303000000000001</v>
+      </c>
+      <c r="L7">
+        <v>45.466000000000001</v>
+      </c>
+      <c r="M7">
+        <v>27.07</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="0"/>
+        <v>24.201000000000001</v>
+      </c>
+      <c r="O7">
+        <v>8.1180000000000003</v>
+      </c>
+      <c r="P7">
+        <v>43.203000000000003</v>
+      </c>
+      <c r="Q7">
+        <v>16.757999999999999</v>
+      </c>
+      <c r="R7">
+        <v>14.238</v>
+      </c>
+      <c r="S7">
+        <v>28.7</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" si="1"/>
+        <v>22.203400000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>1490726379199</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>1490726439173</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <f>(D9-D8)/1000</f>
+        <v>59.973999999999997</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9">
+        <v>59.973999999999997</v>
+      </c>
+      <c r="J9">
+        <v>95.198999999999998</v>
+      </c>
+      <c r="K9">
+        <v>85.840999999999994</v>
+      </c>
+      <c r="L9">
+        <v>57.804000000000002</v>
+      </c>
+      <c r="M9">
+        <v>76.45</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="0"/>
+        <v>75.053599999999989</v>
+      </c>
+      <c r="O9">
+        <v>69.888999999999996</v>
+      </c>
+      <c r="P9">
+        <v>65.087999999999994</v>
+      </c>
+      <c r="Q9">
+        <v>88.17</v>
+      </c>
+      <c r="R9">
+        <v>94.22</v>
+      </c>
+      <c r="S9">
+        <v>38.694000000000003</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="1"/>
+        <v>71.212199999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>1490726445208</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>1490726445228</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <f>(D11-D10)/1000</f>
+        <v>0.02</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>0.02</v>
+      </c>
+      <c r="J11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K11">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="L11">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M11">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="O11">
+        <v>2.7E-2</v>
+      </c>
+      <c r="P11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q11">
+        <v>1.6E-2</v>
+      </c>
+      <c r="R11">
+        <v>0.01</v>
+      </c>
+      <c r="S11">
+        <v>0.01</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>1490726450523</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" s="3">
+        <f>SUM(I3:I11)</f>
+        <v>150.38800000000001</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" ref="J12:M12" si="2">SUM(J3:J11)</f>
+        <v>119.395</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="2"/>
+        <v>110.42400000000001</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="2"/>
+        <v>110.03</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="2"/>
+        <v>110.06399999999999</v>
+      </c>
+      <c r="N12" s="2">
+        <f>SUM(N3:N11)</f>
+        <v>120.06019999999999</v>
+      </c>
+      <c r="O12" s="3">
+        <f>SUM(O3:O11)</f>
+        <v>122.39299999999999</v>
+      </c>
+      <c r="P12" s="3">
+        <f>SUM(P3:P11)</f>
+        <v>114.539</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" ref="Q12:S12" si="3">SUM(Q3:Q11)</f>
+        <v>111.539</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" si="3"/>
+        <v>114.087</v>
+      </c>
+      <c r="S12" s="3">
+        <f t="shared" si="3"/>
+        <v>75.13900000000001</v>
+      </c>
+      <c r="T12" s="2">
+        <f>SUM(T3:T11)</f>
+        <v>107.5394</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
       </c>
       <c r="D14">
         <v>1490726464971</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>1490726465165</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <f>(D15-D14)/1000</f>
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>1490726465222</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <v>1490726471279</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f>(D17-D16)/1000</f>
+        <v>6.0570000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>1490726472591</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>1490726490514</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f>(D19-D18)/1000</f>
+        <v>17.922999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20">
         <v>1490726492536</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>1490726587735</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <f>(D21-D20)/1000</f>
+        <v>95.198999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22">
         <v>1490726597701</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23">
         <v>1490726597723</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <f>(D23-D22)/1000</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24">
         <v>1490726601527</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
       </c>
       <c r="D29">
         <v>1490726610242</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>1490726610445</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <f>(D30-D29)/1000</f>
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31">
         <v>1490726610490</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32">
         <v>1490726616554</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <f>(D32-D31)/1000</f>
+        <v>6.0640000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33">
         <v>1490726616702</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34">
         <v>1490726635005</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <f>(D34-D33)/1000</f>
+        <v>18.303000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35">
         <v>1490726637021</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36">
         <v>1490726722862</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <f>(D36-D35)/1000</f>
+        <v>85.840999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37">
         <v>1490726728879</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38">
         <v>1490726728892</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <f>(D38-D37)/1000</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39">
         <v>1490726732208</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
         <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
       </c>
       <c r="D41">
         <v>1490726753862</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42">
         <v>1490726754069</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <f>(D42-D41)/1000</f>
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <v>1490726754130</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <v>1490726760665</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <f>(D44-D43)/1000</f>
+        <v>6.5350000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D45">
         <v>1490726760793</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>1490726806259</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <f>(D46-D45)/1000</f>
+        <v>45.466000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D47">
         <v>1490726809251</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D48">
         <v>1490726867055</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <f>(D48-D47)/1000</f>
+        <v>57.804000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49">
         <v>1490726873193</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50">
         <v>1490726873211</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <f>(D50-D49)/1000</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D51">
         <v>1490726876432</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
         <v>6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>7</v>
       </c>
       <c r="D53">
         <v>1490726900626</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D54">
         <v>1490726900848</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <f>(D54-D53)/1000</f>
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D55">
         <v>1490726900907</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D56">
         <v>1490726907218</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <f>(D56-D55)/1000</f>
+        <v>6.3109999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57">
         <v>1490726907357</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D58">
         <v>1490726934427</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <f>(D58-D57)/1000</f>
+        <v>27.07</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D59">
         <v>1490726936441</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D60">
         <v>1490727012891</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <f>(D60-D59)/1000</f>
+        <v>76.45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61">
         <v>1490727018907</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D62">
         <v>1490727018918</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <f>(D62-D61)/1000</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D63">
         <v>1490727022016</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
         <v>6</v>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
       </c>
       <c r="D66">
         <v>1490727544702</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67">
         <v>1490727546819</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <f>(D67-D66)/1000</f>
+        <v>2.117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D68">
         <v>1490727546929</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D69">
         <v>1490727589171</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <f>(D69-D68)/1000</f>
+        <v>42.241999999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D70">
         <v>1490727590806</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71">
         <v>1490727598924</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <f>(D71-D70)/1000</f>
+        <v>8.1180000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D72">
         <v>1490727624180</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D73">
         <v>1490727694069</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <f>(D73-D72)/1000</f>
+        <v>69.888999999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D74">
         <v>1490727700387</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D75">
         <v>1490727700414</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <f>(D75-D74)/1000</f>
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D76">
         <v>1490727705739</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
         <v>6</v>
-      </c>
-      <c r="C78" t="s">
-        <v>7</v>
       </c>
       <c r="D78">
         <v>1490727732992</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D79">
         <v>1490727733209</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <f>(D79-D78)/1000</f>
+        <v>0.217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D80">
         <v>1490727733279</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D81">
         <v>1490727739288</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <f>(D81-D80)/1000</f>
+        <v>6.0090000000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D82">
         <v>1490727739442</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D83">
         <v>1490727782645</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <f>(D83-D82)/1000</f>
+        <v>43.203000000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D84">
         <v>1490727784671</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D85">
         <v>1490727849759</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <f>(D85-D84)/1000</f>
+        <v>65.087999999999994</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D86">
         <v>1490727855774</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D87">
         <v>1490727855796</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <f>(D87-D86)/1000</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D88">
         <v>1490727859036</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" t="s">
         <v>6</v>
-      </c>
-      <c r="C90" t="s">
-        <v>7</v>
       </c>
       <c r="D90">
         <v>1490727881032</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D91">
         <v>1490727881312</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <f>(D91-D90)/1000</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D92">
         <v>1490727881369</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D93">
         <v>1490727887684</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <f>(D93-D92)/1000</f>
+        <v>6.3150000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D94">
         <v>1490727887805</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D95">
         <v>1490727904563</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <f>(D95-D94)/1000</f>
+        <v>16.757999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D96">
         <v>1490727909432</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D97">
         <v>1490727997602</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <f>(D97-D96)/1000</f>
+        <v>88.17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D98">
         <v>1490728003617</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D99">
         <v>1490728003633</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <f>(D99-D98)/1000</f>
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B100" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D100">
         <v>1490728006652</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
         <v>6</v>
-      </c>
-      <c r="C102" t="s">
-        <v>7</v>
       </c>
       <c r="D102">
         <v>1490728014501</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D103">
         <v>1490728014676</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <f>(D103-D102)/1000</f>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D104">
         <v>1490728014724</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D105">
         <v>1490728020168</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <f>(D105-D104)/1000</f>
+        <v>5.444</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D106">
         <v>1490728020302</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D107">
         <v>1490728034540</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <f>(D107-D106)/1000</f>
+        <v>14.238</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D108">
         <v>1490728036553</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D109">
         <v>1490728130773</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <f>(D109-D108)/1000</f>
+        <v>94.22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D110">
         <v>1490728136794</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D111">
         <v>1490728136804</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <f>(D111-D110)/1000</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D112">
         <v>1490728139767</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" t="s">
         <v>6</v>
-      </c>
-      <c r="C114" t="s">
-        <v>7</v>
       </c>
       <c r="D114">
         <v>1490728156534</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D115">
         <v>1490728156699</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <f>(D115-D114)/1000</f>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B116" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D116">
         <v>1490728156754</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D117">
         <v>1490728164324</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <f>(D117-D116)/1000</f>
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D118">
         <v>1490728164440</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D119">
         <v>1490728193140</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <f>(D119-D118)/1000</f>
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B120" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D120">
         <v>1490728219097</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D121">
         <v>1490728257791</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <f>(D121-D120)/1000</f>
+        <v>38.694000000000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D122">
         <v>1490728263817</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D123">
         <v>1490728263827</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <f>(D123-D122)/1000</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B124" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D124">
         <v>1490728266670</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>